<commit_message>
Zoe submit six scripts
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/TST1131_ViewsMoveDevicesApartFromAllDevicesView.xlsx
+++ b/NformTester/NformTester/Keywordscripts/TST1131_ViewsMoveDevicesApartFromAllDevicesView.xlsx
@@ -1255,7 +1255,7 @@
     <definedName name="VerifyTxtfileValues">'Form DataValDepend'!$CH$1</definedName>
     <definedName name="VerifyTxtfileValuesCol">'Form DataValDepend'!$CH:$CH</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -3887,7 +3887,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3895,34 +3895,34 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3930,7 +3930,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -4152,10 +4152,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
     <cellStyle name="常规 2 2" xfId="3"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -4178,7 +4178,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4464,24 +4464,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.75" style="19" customWidth="1"/>
+    <col min="2" max="2" width="28.375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="29.75" customWidth="1"/>
+    <col min="6" max="6" width="29.25" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="34.140625" customWidth="1"/>
-    <col min="9" max="9" width="31.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="34.125" customWidth="1"/>
+    <col min="9" max="9" width="31.875" customWidth="1"/>
+    <col min="11" max="11" width="10.125" customWidth="1"/>
+    <col min="12" max="12" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25.5">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>818</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="15">
       <c r="A2" s="2" t="s">
         <v>820</v>
       </c>
@@ -4611,7 +4611,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="17"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" ht="15">
       <c r="A5" s="2" t="s">
         <v>826</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="M6" s="3"/>
       <c r="N6" s="17"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="15">
       <c r="A7" s="2" t="s">
         <v>803</v>
       </c>
@@ -4961,7 +4961,7 @@
       <c r="N16" s="22"/>
       <c r="O16" s="20"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" ht="15">
       <c r="A17" s="25" t="s">
         <v>811</v>
       </c>
@@ -5388,7 +5388,7 @@
       <c r="N31" s="17"/>
       <c r="O31" s="20"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" ht="15">
       <c r="C32" s="3">
         <v>31</v>
       </c>
@@ -5605,7 +5605,7 @@
       <c r="M40" s="3"/>
       <c r="N40" s="17"/>
     </row>
-    <row r="41" spans="3:15" ht="16.5">
+    <row r="41" spans="3:15" ht="14.25">
       <c r="C41" s="3">
         <v>40</v>
       </c>
@@ -5915,7 +5915,7 @@
       <c r="M60" s="3"/>
       <c r="N60" s="17"/>
     </row>
-    <row r="61" spans="3:14">
+    <row r="61" spans="3:14" ht="15">
       <c r="C61" s="3"/>
       <c r="D61" s="14"/>
       <c r="E61" s="3"/>
@@ -6181,7 +6181,7 @@
       <c r="M79" s="3"/>
       <c r="N79" s="17"/>
     </row>
-    <row r="80" spans="3:14">
+    <row r="80" spans="3:14" ht="15">
       <c r="C80" s="3"/>
       <c r="D80" s="14"/>
       <c r="E80" s="3"/>
@@ -6433,7 +6433,7 @@
       <c r="M97" s="3"/>
       <c r="N97" s="17"/>
     </row>
-    <row r="98" spans="3:14">
+    <row r="98" spans="3:14" ht="15">
       <c r="C98" s="3"/>
       <c r="D98" s="14"/>
       <c r="E98" s="3"/>
@@ -6685,7 +6685,7 @@
       <c r="M115" s="3"/>
       <c r="N115" s="17"/>
     </row>
-    <row r="116" spans="3:14">
+    <row r="116" spans="3:14" ht="15">
       <c r="C116" s="3"/>
       <c r="D116" s="14"/>
       <c r="E116" s="5"/>
@@ -6755,7 +6755,7 @@
       <c r="M120" s="3"/>
       <c r="N120" s="17"/>
     </row>
-    <row r="121" spans="3:14" ht="16.5">
+    <row r="121" spans="3:14" ht="14.25">
       <c r="C121" s="3"/>
       <c r="D121" s="12"/>
       <c r="E121" s="5"/>
@@ -6811,7 +6811,7 @@
       <c r="M124" s="3"/>
       <c r="N124" s="17"/>
     </row>
-    <row r="125" spans="3:14" ht="16.5">
+    <row r="125" spans="3:14" ht="14.25">
       <c r="C125" s="3"/>
       <c r="D125" s="12"/>
       <c r="E125" s="5"/>
@@ -6980,7 +6980,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:85">
       <c r="A1" t="s">
@@ -10889,7 +10889,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:1066">
       <c r="A1" t="s">
@@ -29949,10 +29949,10 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>